<commit_message>
sắp hết rồi cố lên
</commit_message>
<xml_diff>
--- a/src/test/resources/datatest/Crm.xlsx
+++ b/src/test/resources/datatest/Crm.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
   <si>
     <t>EMAIL</t>
   </si>
@@ -90,9 +90,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -408,7 +411,7 @@
       <c r="B2">
         <v>123456</v>
       </c>
-      <c r="C2" t="s" s="2">
+      <c r="C2" t="s" s="3">
         <v>5</v>
       </c>
     </row>

</xml_diff>